<commit_message>
updated BU plan because of mistake
</commit_message>
<xml_diff>
--- a/MicrowaveOvenSolution/diagrammer/Bottom-up Plan Microwave.xlsx
+++ b/MicrowaveOvenSolution/diagrammer/Bottom-up Plan Microwave.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mabui\Desktop\SWT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mabui\Desktop\IKT\SWT\MicrowaveOvenSolution\diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" xr2:uid="{80901D84-10AB-42CD-A292-219F37A6ACB6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5625"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>Step</t>
   </si>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -329,9 +329,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Kontrollér celle" xfId="2" builtinId="23"/>
+    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Overskrift 2" xfId="1" builtinId="17"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -347,9 +347,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -387,7 +387,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -493,7 +493,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -642,29 +642,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8057CB-E847-4082-8786-69D77E578501}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K7"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -696,7 +696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -714,7 +714,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="2:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>2</v>
       </c>
@@ -732,7 +732,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="2:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -750,15 +750,13 @@
       <c r="J5" s="4"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="2:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>4</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
@@ -776,7 +774,7 @@
       </c>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="2:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>5</v>
       </c>

</xml_diff>